<commit_message>
index.html and nano set up
</commit_message>
<xml_diff>
--- a/doku/userstories/Userstories.xlsx
+++ b/doku/userstories/Userstories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">möchte ich ein Zertifikate ändern können, falls Daten aktualisiert werden müssen. </t>
+  </si>
+  <si>
+    <t>US1</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,6 +428,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>

</xml_diff>